<commit_message>
Updated the sensitivity analysis
</commit_message>
<xml_diff>
--- a/Sensitivity Analysis.xlsx
+++ b/Sensitivity Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eashwar\Desktop\ENSE\ENSE622\Final Exam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782F7B3E-668B-4A30-A8F4-2ED34A251B07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7940711F-7C42-41E9-A04F-DB23255869B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0352C288-3703-4171-8A0F-C906E828E2CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="89">
   <si>
     <t>Low =&gt; Good</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Vc</t>
   </si>
   <si>
-    <t>Factor Uncertainties Table for Design 4</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>MAVF Analysis Table for Design 4 for unceretainties in Cost (C), Tech Value (T), Rc and Rtv</t>
-  </si>
-  <si>
     <t>When Cost is Low</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>When Rc is High</t>
   </si>
   <si>
-    <t>MAVF Single Factor Uncertainty table for Design Factor 4</t>
-  </si>
-  <si>
     <t>Low Fi</t>
   </si>
   <si>
@@ -294,6 +285,24 @@
   </si>
   <si>
     <t>Rmft</t>
+  </si>
+  <si>
+    <t>Sensitivity Analysis Part - A</t>
+  </si>
+  <si>
+    <t>Sensitivity Analysis Part - B</t>
+  </si>
+  <si>
+    <t>Factor Uncertainties Table for Design  Factors</t>
+  </si>
+  <si>
+    <t>Factor Uncertainties Table for Ranks</t>
+  </si>
+  <si>
+    <t>MAVF values from Sensitivity Analysis-B</t>
+  </si>
+  <si>
+    <t>MAVF values from Sensitivity Analysis-A</t>
   </si>
 </sst>
 </file>
@@ -656,7 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -683,7 +692,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -700,12 +708,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -867,26 +869,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2451,10 +2455,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2590800" cy="676275"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2472,7 +2476,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17506950" y="4419600"/>
+              <a:off x="22774275" y="5305425"/>
               <a:ext cx="2590800" cy="676275"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2572,7 +2576,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17506950" y="4419600"/>
+              <a:off x="22774275" y="5305425"/>
               <a:ext cx="2590800" cy="676275"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2617,16 +2621,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>552449</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2655,10 +2659,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2590800" cy="723899"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2676,7 +2680,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17573625" y="5210175"/>
+              <a:off x="22783800" y="6076950"/>
               <a:ext cx="2590800" cy="723899"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2776,7 +2780,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17573625" y="5210175"/>
+              <a:off x="22783800" y="6076950"/>
               <a:ext cx="2590800" cy="723899"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2821,12 +2825,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1390650</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2667000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6810375" cy="723900"/>
+    <xdr:ext cx="6915150" cy="1971675"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -2842,8 +2846,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17287875" y="7696200"/>
-              <a:ext cx="6810375" cy="723900"/>
+              <a:off x="20164425" y="7658100"/>
+              <a:ext cx="6915150" cy="1971675"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3197,8 +3201,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17287875" y="7696200"/>
-              <a:ext cx="6810375" cy="723900"/>
+              <a:off x="20164425" y="7658100"/>
+              <a:ext cx="6915150" cy="1971675"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3254,10 +3258,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2590800" cy="723899"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3275,7 +3279,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17687925" y="6829425"/>
+              <a:off x="22860000" y="7591425"/>
               <a:ext cx="2590800" cy="723899"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3375,7 +3379,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17687925" y="6829425"/>
+              <a:off x="22860000" y="7591425"/>
               <a:ext cx="2590800" cy="723899"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3420,10 +3424,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2590800" cy="723899"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3441,7 +3445,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17697450" y="6124575"/>
+              <a:off x="22802850" y="6877050"/>
               <a:ext cx="2590800" cy="723899"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3541,7 +3545,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="17697450" y="6124575"/>
+              <a:off x="22802850" y="6877050"/>
               <a:ext cx="2590800" cy="723899"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3955,10 +3959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E092A5B7-1CD1-4569-A0AD-62083D236086}">
-  <dimension ref="A1:S90"/>
+  <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3981,40 +3985,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="A1" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="49"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -4023,74 +4027,74 @@
       <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>44</v>
-      </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="54"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="46" t="s">
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="47" t="s">
-        <v>40</v>
+      <c r="K3" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="44" t="s">
+        <v>37</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="58" t="s">
+      <c r="R3" s="55" t="s">
         <v>8</v>
       </c>
       <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="23">
-        <v>100</v>
-      </c>
-      <c r="C4" s="23">
-        <v>100</v>
-      </c>
-      <c r="D4" s="23">
+        <v>33</v>
+      </c>
+      <c r="B4" s="20">
+        <v>100</v>
+      </c>
+      <c r="C4" s="20">
+        <v>100</v>
+      </c>
+      <c r="D4" s="20">
         <v>100</v>
       </c>
       <c r="E4" s="5">
         <v>100</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
+      <c r="G4" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
       <c r="J4" s="5">
         <v>100</v>
       </c>
@@ -4104,13 +4108,13 @@
         <v>100</v>
       </c>
       <c r="N4" s="4"/>
-      <c r="O4" s="23" t="s">
+      <c r="O4" s="20" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="3">
         <v>25</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="20" t="s">
         <v>10</v>
       </c>
       <c r="R4" s="5">
@@ -4121,26 +4125,26 @@
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="23">
-        <v>100</v>
-      </c>
-      <c r="C5" s="23">
-        <v>100</v>
-      </c>
-      <c r="D5" s="23">
+        <v>34</v>
+      </c>
+      <c r="B5" s="20">
+        <v>100</v>
+      </c>
+      <c r="C5" s="20">
+        <v>100</v>
+      </c>
+      <c r="D5" s="20">
         <v>100</v>
       </c>
       <c r="E5" s="5">
         <v>100</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
+      <c r="G5" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="5">
         <v>100</v>
       </c>
@@ -4154,14 +4158,14 @@
         <v>100</v>
       </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="23" t="s">
-        <v>53</v>
+      <c r="O5" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="P5" s="3">
         <v>25</v>
       </c>
-      <c r="Q5" s="23" t="s">
-        <v>56</v>
+      <c r="Q5" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="R5" s="5">
         <f xml:space="preserve"> P5/(P5+P8)</f>
@@ -4171,26 +4175,26 @@
     </row>
     <row r="6" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="23">
-        <v>100</v>
-      </c>
-      <c r="C6" s="23">
-        <v>100</v>
-      </c>
-      <c r="D6" s="23">
+        <v>35</v>
+      </c>
+      <c r="B6" s="20">
+        <v>100</v>
+      </c>
+      <c r="C6" s="20">
+        <v>100</v>
+      </c>
+      <c r="D6" s="20">
         <v>100</v>
       </c>
       <c r="E6" s="5">
         <v>100</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="G6" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="5">
         <v>100</v>
       </c>
@@ -4204,14 +4208,14 @@
         <v>100</v>
       </c>
       <c r="N6" s="4"/>
-      <c r="O6" s="23" t="s">
-        <v>54</v>
+      <c r="O6" s="20" t="s">
+        <v>51</v>
       </c>
       <c r="P6" s="3">
         <v>25</v>
       </c>
-      <c r="Q6" s="23" t="s">
-        <v>57</v>
+      <c r="Q6" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="R6" s="5">
         <f xml:space="preserve"> P6/(P6+P8)</f>
@@ -4221,7 +4225,7 @@
     </row>
     <row r="7" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7" s="7">
         <v>100</v>
@@ -4236,11 +4240,11 @@
         <v>100</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="G7" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
       <c r="J7" s="5">
         <v>100</v>
       </c>
@@ -4254,14 +4258,14 @@
         <v>100</v>
       </c>
       <c r="N7" s="4"/>
-      <c r="O7" s="23" t="s">
-        <v>55</v>
+      <c r="O7" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="P7" s="6">
         <v>25</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="R7" s="8">
         <f xml:space="preserve"> P7/(P7+P8)</f>
@@ -4270,17 +4274,17 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="G8" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="5">
         <v>100</v>
       </c>
@@ -4293,28 +4297,28 @@
       <c r="M8" s="5">
         <v>100</v>
       </c>
-      <c r="O8" s="29" t="s">
+      <c r="O8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="29">
-        <v>100</v>
-      </c>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
+      <c r="P8" s="26">
+        <v>100</v>
+      </c>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="G9" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="5">
         <v>100</v>
       </c>
@@ -4332,17 +4336,17 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="G10" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="5">
         <v>100</v>
       </c>
@@ -4366,11 +4370,11 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="G11" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5">
         <v>100</v>
       </c>
@@ -4383,11 +4387,11 @@
       <c r="M11" s="5">
         <v>100</v>
       </c>
-      <c r="Q11" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
+      <c r="Q11" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
     </row>
     <row r="12" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
@@ -4396,11 +4400,11 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="G12" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5">
         <v>100</v>
       </c>
@@ -4416,11 +4420,11 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
+      <c r="Q12" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -4429,11 +4433,11 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="G13" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5">
         <v>100</v>
       </c>
@@ -4449,11 +4453,11 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="35" t="s">
+      <c r="Q13" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
     </row>
     <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
@@ -4462,11 +4466,11 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="G14" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5">
         <v>100</v>
       </c>
@@ -4482,11 +4486,11 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="35" t="s">
+      <c r="Q14" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
     </row>
     <row r="15" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -4495,11 +4499,11 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
       <c r="J15" s="5">
         <v>100</v>
       </c>
@@ -4515,11 +4519,11 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="35" t="s">
+      <c r="Q15" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
     </row>
     <row r="16" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
@@ -4528,11 +4532,11 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
+      <c r="G16" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="8">
         <v>100</v>
       </c>
@@ -4548,11 +4552,11 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="R16" s="34"/>
-      <c r="S16" s="34"/>
+      <c r="Q16" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
     </row>
     <row r="17" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
@@ -4561,8 +4565,8 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -4570,245 +4574,234 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
+      <c r="Q17" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
     </row>
     <row r="18" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="62"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="59"/>
       <c r="M18" s="1"/>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
+      <c r="Q18" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
     </row>
     <row r="19" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20">
         <f>(P4)/(P4+P5)</f>
         <v>0.5</v>
       </c>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
     </row>
     <row r="21" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="60" t="s">
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="60"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
+      <c r="K21" s="57"/>
     </row>
     <row r="22" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="16" t="s">
+      <c r="G22" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="I22" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="J22" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22" s="64"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
+      <c r="J22" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="K22" s="61"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
     </row>
     <row r="23" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="23">
-        <v>100</v>
-      </c>
-      <c r="C23" s="23">
-        <v>100</v>
-      </c>
-      <c r="D23" s="23">
-        <v>100</v>
-      </c>
-      <c r="E23" s="23">
-        <v>100</v>
-      </c>
-      <c r="F23" s="23">
+        <v>33</v>
+      </c>
+      <c r="B23" s="20">
+        <v>100</v>
+      </c>
+      <c r="C23" s="20">
+        <v>100</v>
+      </c>
+      <c r="D23" s="20">
+        <v>100</v>
+      </c>
+      <c r="E23" s="20">
+        <v>100</v>
+      </c>
+      <c r="F23" s="20">
         <f xml:space="preserve"> (B9 - B23)/(B9 - B4)</f>
         <v>1</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="60">
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="57">
         <f>SUM(F20*F23,K20*K23)</f>
         <v>0.5</v>
       </c>
-      <c r="K23" s="60"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
+      <c r="K23" s="57"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="28"/>
     </row>
     <row r="24" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="23">
-        <v>100</v>
-      </c>
-      <c r="C24" s="23">
-        <v>100</v>
-      </c>
-      <c r="D24" s="23">
-        <v>100</v>
-      </c>
-      <c r="E24" s="23">
-        <v>100</v>
-      </c>
-      <c r="F24" s="23">
+        <v>34</v>
+      </c>
+      <c r="B24" s="20">
+        <v>100</v>
+      </c>
+      <c r="C24" s="20">
+        <v>100</v>
+      </c>
+      <c r="D24" s="20">
+        <v>100</v>
+      </c>
+      <c r="E24" s="20">
+        <v>100</v>
+      </c>
+      <c r="F24" s="20">
         <f xml:space="preserve"> (B9 - B24)/(B9 - B4)</f>
         <v>1</v>
       </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="60">
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="57">
         <f>SUM(F20*F24,K20*K24)</f>
         <v>0.5</v>
       </c>
-      <c r="K24" s="60"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
+      <c r="K24" s="57"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
     </row>
     <row r="25" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="23">
-        <v>100</v>
-      </c>
-      <c r="C25" s="23">
-        <v>100</v>
-      </c>
-      <c r="D25" s="23">
-        <v>100</v>
-      </c>
-      <c r="E25" s="23">
-        <v>100</v>
-      </c>
-      <c r="F25" s="23">
+        <v>35</v>
+      </c>
+      <c r="B25" s="20">
+        <v>100</v>
+      </c>
+      <c r="C25" s="20">
+        <v>100</v>
+      </c>
+      <c r="D25" s="20">
+        <v>100</v>
+      </c>
+      <c r="E25" s="20">
+        <v>100</v>
+      </c>
+      <c r="F25" s="20">
         <f xml:space="preserve"> (B9 - B25)/(B9 - B4)</f>
         <v>1</v>
       </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="60">
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="57">
         <f>SUM(F20*F25,K20*K25)</f>
         <v>0.5</v>
       </c>
-      <c r="K25" s="60"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
+      <c r="K25" s="57"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="28"/>
     </row>
     <row r="26" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26" s="7">
         <v>100</v>
@@ -4828,322 +4821,341 @@
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="45">
+      <c r="I26" s="54"/>
+      <c r="J26" s="42">
         <f>SUM(F20*F26,K20*K26)</f>
         <v>0.5</v>
       </c>
-      <c r="K26" s="61"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
+      <c r="K26" s="58"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
     </row>
     <row r="27" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
     </row>
     <row r="28" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
     </row>
     <row r="29" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="31"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-    </row>
-    <row r="33" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="48" t="s">
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+    </row>
+    <row r="33" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="68"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+    </row>
+    <row r="34" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="51"/>
+      <c r="C34" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
-    </row>
-    <row r="34" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="53" t="s">
+      <c r="D34" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="72" t="s">
+      <c r="H34" s="51"/>
+      <c r="I34" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="73" t="s">
+      <c r="K34" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
-    </row>
-    <row r="35" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="65" t="s">
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+    </row>
+    <row r="35" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="66"/>
-      <c r="C35" s="23">
+      <c r="B35" s="63"/>
+      <c r="C35" s="20">
         <v>30</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="20">
         <v>30</v>
       </c>
       <c r="E35" s="5">
         <v>30</v>
       </c>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="31"/>
-    </row>
-    <row r="36" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="66"/>
-      <c r="C36" s="23">
+      <c r="G35" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="63"/>
+      <c r="I35" s="20">
         <v>30</v>
       </c>
-      <c r="D36" s="23">
+      <c r="J35" s="20">
+        <v>30</v>
+      </c>
+      <c r="K35" s="5">
+        <v>30</v>
+      </c>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="28"/>
+      <c r="Q35" s="28"/>
+      <c r="R35" s="28"/>
+    </row>
+    <row r="36" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="63"/>
+      <c r="C36" s="20">
+        <v>30</v>
+      </c>
+      <c r="D36" s="20">
         <v>30</v>
       </c>
       <c r="E36" s="5">
         <v>30</v>
       </c>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="31"/>
-    </row>
-    <row r="37" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="66"/>
-      <c r="C37" s="23">
+      <c r="G36" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="63"/>
+      <c r="I36" s="20">
         <v>30</v>
       </c>
-      <c r="D37" s="23">
+      <c r="J36" s="20">
+        <v>30</v>
+      </c>
+      <c r="K36" s="5">
+        <v>30</v>
+      </c>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="28"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="28"/>
+    </row>
+    <row r="37" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="63"/>
+      <c r="C37" s="20">
+        <v>30</v>
+      </c>
+      <c r="D37" s="20">
         <v>30</v>
       </c>
       <c r="E37" s="5">
         <v>30</v>
       </c>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="L37" s="31"/>
-      <c r="M37" s="31"/>
-      <c r="N37" s="31"/>
-      <c r="O37" s="31"/>
-      <c r="P37" s="31"/>
-    </row>
-    <row r="38" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="66"/>
-      <c r="C38" s="23">
+      <c r="G37" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" s="63"/>
+      <c r="I37" s="20">
         <v>30</v>
       </c>
-      <c r="D38" s="23">
+      <c r="J37" s="20">
         <v>30</v>
       </c>
-      <c r="E38" s="5">
+      <c r="K37" s="5">
         <v>30</v>
       </c>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="31"/>
-      <c r="O38" s="31"/>
-      <c r="P38" s="31"/>
-    </row>
-    <row r="39" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="66"/>
-      <c r="C39" s="23">
+      <c r="M37" s="28"/>
+      <c r="N37" s="28"/>
+      <c r="O37" s="28"/>
+      <c r="P37" s="28"/>
+      <c r="Q37" s="28"/>
+      <c r="R37" s="28"/>
+    </row>
+    <row r="38" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="65"/>
+      <c r="C38" s="7">
         <v>30</v>
       </c>
-      <c r="D39" s="23">
+      <c r="D38" s="7">
         <v>30</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E38" s="8">
         <v>30</v>
       </c>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="L39" s="28"/>
+      <c r="G38" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="65"/>
+      <c r="I38" s="7">
+        <v>30</v>
+      </c>
+      <c r="J38" s="7">
+        <v>30</v>
+      </c>
+      <c r="K38" s="8">
+        <v>30</v>
+      </c>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="28"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="28"/>
+    </row>
+    <row r="39" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F39" s="20"/>
+      <c r="L39" s="25"/>
       <c r="M39" s="28"/>
       <c r="N39" s="28"/>
       <c r="O39" s="28"/>
       <c r="P39" s="28"/>
-    </row>
-    <row r="40" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="66"/>
-      <c r="C40" s="23">
-        <v>30</v>
-      </c>
-      <c r="D40" s="23">
-        <v>30</v>
-      </c>
-      <c r="E40" s="5">
-        <v>30</v>
-      </c>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="L40" s="28"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
+    </row>
+    <row r="40" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F40" s="20"/>
+      <c r="L40" s="25"/>
       <c r="M40" s="28"/>
       <c r="N40" s="28"/>
       <c r="O40" s="28"/>
       <c r="P40" s="28"/>
-    </row>
-    <row r="41" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="66"/>
-      <c r="C41" s="23">
-        <v>30</v>
-      </c>
-      <c r="D41" s="23">
-        <v>30</v>
-      </c>
-      <c r="E41" s="5">
-        <v>30</v>
-      </c>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="L41" s="28"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
+    </row>
+    <row r="41" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F41" s="20"/>
+      <c r="L41" s="25"/>
       <c r="M41" s="28"/>
       <c r="N41" s="28"/>
       <c r="O41" s="28"/>
       <c r="P41" s="28"/>
-    </row>
-    <row r="42" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="68"/>
-      <c r="C42" s="7">
-        <v>30</v>
-      </c>
-      <c r="D42" s="7">
-        <v>30</v>
-      </c>
-      <c r="E42" s="8">
-        <v>30</v>
-      </c>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28"/>
-      <c r="O42" s="28"/>
-      <c r="P42" s="28"/>
-    </row>
-    <row r="43" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="59"/>
-      <c r="B43" s="59"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="28"/>
-      <c r="N43" s="28"/>
-      <c r="O43" s="28"/>
-      <c r="P43" s="28"/>
-    </row>
-    <row r="44" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Q41" s="28"/>
+      <c r="R41" s="28"/>
+    </row>
+    <row r="42" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F42" s="20"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="25"/>
+    </row>
+    <row r="43" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="56"/>
+      <c r="B43" s="56"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+      <c r="O43" s="25"/>
+      <c r="P43" s="25"/>
+    </row>
+    <row r="44" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -5153,7 +5165,7 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -5163,1229 +5175,1394 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="11"/>
+    <row r="46" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="10"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" s="12"/>
-      <c r="Q46" s="74"/>
-    </row>
-    <row r="47" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="14"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="23"/>
-      <c r="M47" s="23"/>
-      <c r="N47" s="23"/>
-      <c r="O47" s="23"/>
-      <c r="P47" s="56"/>
-      <c r="Q47" s="75"/>
-    </row>
-    <row r="48" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="53" t="s">
+      <c r="J46" s="11"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="71"/>
+    </row>
+    <row r="47" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="13"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="72"/>
+    </row>
+    <row r="48" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="54"/>
-      <c r="C48" s="16" t="s">
+      <c r="B48" s="51"/>
+      <c r="C48" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E48" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I48" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F48" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G48" s="16" t="s">
+      <c r="J48" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="K48" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L48" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N48" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="O48" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="P48" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q48" s="61"/>
+    </row>
+    <row r="49" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="39"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="74">
+        <v>0</v>
+      </c>
+      <c r="E49" s="74">
+        <v>0</v>
+      </c>
+      <c r="F49" s="74">
+        <v>0</v>
+      </c>
+      <c r="G49" s="74">
+        <v>0</v>
+      </c>
+      <c r="H49" s="74">
+        <v>0</v>
+      </c>
+      <c r="I49" s="74">
+        <v>0</v>
+      </c>
+      <c r="J49" s="74">
+        <v>0</v>
+      </c>
+      <c r="K49" s="74">
+        <v>0</v>
+      </c>
+      <c r="L49" s="74">
+        <v>0</v>
+      </c>
+      <c r="M49" s="74">
+        <v>0</v>
+      </c>
+      <c r="N49" s="74">
+        <v>0</v>
+      </c>
+      <c r="O49" s="74">
+        <v>0</v>
+      </c>
+      <c r="P49" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="39"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="74">
+        <v>0</v>
+      </c>
+      <c r="E50" s="74">
+        <v>0</v>
+      </c>
+      <c r="F50" s="74">
+        <v>0</v>
+      </c>
+      <c r="G50" s="74">
+        <v>0</v>
+      </c>
+      <c r="H50" s="74">
+        <v>0</v>
+      </c>
+      <c r="I50" s="74">
+        <v>0</v>
+      </c>
+      <c r="J50" s="74">
+        <v>0</v>
+      </c>
+      <c r="K50" s="74">
+        <v>0</v>
+      </c>
+      <c r="L50" s="74">
+        <v>0</v>
+      </c>
+      <c r="M50" s="74">
+        <v>0</v>
+      </c>
+      <c r="N50" s="74">
+        <v>0</v>
+      </c>
+      <c r="O50" s="74">
+        <v>0</v>
+      </c>
+      <c r="P50" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="39"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="74">
+        <v>0</v>
+      </c>
+      <c r="E51" s="74">
+        <v>0</v>
+      </c>
+      <c r="F51" s="74">
+        <v>0</v>
+      </c>
+      <c r="G51" s="74">
+        <v>0</v>
+      </c>
+      <c r="H51" s="74">
+        <v>0</v>
+      </c>
+      <c r="I51" s="74">
+        <v>0</v>
+      </c>
+      <c r="J51" s="74">
+        <v>0</v>
+      </c>
+      <c r="K51" s="74">
+        <v>0</v>
+      </c>
+      <c r="L51" s="74">
+        <v>0</v>
+      </c>
+      <c r="M51" s="74">
+        <v>0</v>
+      </c>
+      <c r="N51" s="74">
+        <v>0</v>
+      </c>
+      <c r="O51" s="74">
+        <v>0</v>
+      </c>
+      <c r="P51" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="39"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="74">
+        <v>0</v>
+      </c>
+      <c r="E52" s="74">
+        <v>0</v>
+      </c>
+      <c r="F52" s="74">
+        <v>0</v>
+      </c>
+      <c r="G52" s="74">
+        <v>0</v>
+      </c>
+      <c r="H52" s="74">
+        <v>0</v>
+      </c>
+      <c r="I52" s="74">
+        <v>0</v>
+      </c>
+      <c r="J52" s="74">
+        <v>0</v>
+      </c>
+      <c r="K52" s="74">
+        <v>0</v>
+      </c>
+      <c r="L52" s="74">
+        <v>0</v>
+      </c>
+      <c r="M52" s="74">
+        <v>0</v>
+      </c>
+      <c r="N52" s="74">
+        <v>0</v>
+      </c>
+      <c r="O52" s="74">
+        <v>0</v>
+      </c>
+      <c r="P52" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="39"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="74">
+        <v>0</v>
+      </c>
+      <c r="E53" s="74">
+        <v>0</v>
+      </c>
+      <c r="F53" s="74">
+        <v>0</v>
+      </c>
+      <c r="G53" s="74">
+        <v>0</v>
+      </c>
+      <c r="H53" s="74">
+        <v>0</v>
+      </c>
+      <c r="I53" s="74">
+        <v>0</v>
+      </c>
+      <c r="J53" s="74">
+        <v>0</v>
+      </c>
+      <c r="K53" s="74">
+        <v>0</v>
+      </c>
+      <c r="L53" s="74">
+        <v>0</v>
+      </c>
+      <c r="M53" s="74">
+        <v>0</v>
+      </c>
+      <c r="N53" s="74">
+        <v>0</v>
+      </c>
+      <c r="O53" s="74">
+        <v>0</v>
+      </c>
+      <c r="P53" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="39"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="74">
+        <v>0</v>
+      </c>
+      <c r="E54" s="74">
+        <v>0</v>
+      </c>
+      <c r="F54" s="74">
+        <v>0</v>
+      </c>
+      <c r="G54" s="74">
+        <v>0</v>
+      </c>
+      <c r="H54" s="74">
+        <v>0</v>
+      </c>
+      <c r="I54" s="74">
+        <v>0</v>
+      </c>
+      <c r="J54" s="74">
+        <v>0</v>
+      </c>
+      <c r="K54" s="74">
+        <v>0</v>
+      </c>
+      <c r="L54" s="74">
+        <v>0</v>
+      </c>
+      <c r="M54" s="74">
+        <v>0</v>
+      </c>
+      <c r="N54" s="74">
+        <v>0</v>
+      </c>
+      <c r="O54" s="74">
+        <v>0</v>
+      </c>
+      <c r="P54" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="39"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="74">
+        <v>0</v>
+      </c>
+      <c r="E55" s="74">
+        <v>0</v>
+      </c>
+      <c r="F55" s="74">
+        <v>0</v>
+      </c>
+      <c r="G55" s="74">
+        <v>0</v>
+      </c>
+      <c r="H55" s="74">
+        <v>0</v>
+      </c>
+      <c r="I55" s="74">
+        <v>0</v>
+      </c>
+      <c r="J55" s="74">
+        <v>0</v>
+      </c>
+      <c r="K55" s="74">
+        <v>0</v>
+      </c>
+      <c r="L55" s="74">
+        <v>0</v>
+      </c>
+      <c r="M55" s="74">
+        <v>0</v>
+      </c>
+      <c r="N55" s="74">
+        <v>0</v>
+      </c>
+      <c r="O55" s="74">
+        <v>0</v>
+      </c>
+      <c r="P55" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="42"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="76">
+        <v>0</v>
+      </c>
+      <c r="E56" s="76">
+        <v>0</v>
+      </c>
+      <c r="F56" s="76">
+        <v>0</v>
+      </c>
+      <c r="G56" s="76">
+        <v>0</v>
+      </c>
+      <c r="H56" s="76">
+        <v>0</v>
+      </c>
+      <c r="I56" s="76">
+        <v>0</v>
+      </c>
+      <c r="J56" s="76">
+        <v>0</v>
+      </c>
+      <c r="K56" s="76">
+        <v>0</v>
+      </c>
+      <c r="L56" s="76">
+        <v>0</v>
+      </c>
+      <c r="M56" s="76">
+        <v>0</v>
+      </c>
+      <c r="N56" s="76">
+        <v>0</v>
+      </c>
+      <c r="O56" s="76">
+        <v>0</v>
+      </c>
+      <c r="P56" s="76">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="3"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="74"/>
+      <c r="F57" s="74"/>
+      <c r="G57" s="74"/>
+      <c r="H57" s="74"/>
+      <c r="I57" s="74"/>
+      <c r="J57" s="74"/>
+      <c r="K57" s="74"/>
+      <c r="L57" s="74"/>
+      <c r="M57" s="74"/>
+      <c r="N57" s="74"/>
+      <c r="O57" s="74"/>
+      <c r="P57" s="74"/>
+      <c r="Q57" s="74"/>
+    </row>
+    <row r="58" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="3"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="74"/>
+      <c r="I58" s="74"/>
+      <c r="J58" s="74"/>
+      <c r="K58" s="74"/>
+      <c r="L58" s="74"/>
+      <c r="M58" s="74"/>
+      <c r="N58" s="74"/>
+      <c r="O58" s="74"/>
+      <c r="P58" s="74"/>
+      <c r="Q58" s="74"/>
+    </row>
+    <row r="59" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="H48" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="I48" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="J48" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="K48" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="L48" s="16" t="s">
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="85"/>
+      <c r="J59" s="85"/>
+      <c r="K59" s="85"/>
+      <c r="L59" s="85"/>
+      <c r="M59" s="85"/>
+      <c r="N59" s="85"/>
+      <c r="O59" s="85"/>
+      <c r="P59" s="85"/>
+      <c r="Q59" s="86"/>
+    </row>
+    <row r="60" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="51"/>
+      <c r="C60" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G60" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="I60" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="J60" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="K60" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L60" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M48" s="16" t="s">
+      <c r="M60" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N60" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="O60" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="P60" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q60" s="61"/>
+    </row>
+    <row r="61" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="39"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="74">
+        <v>0</v>
+      </c>
+      <c r="E61" s="74">
+        <v>0</v>
+      </c>
+      <c r="F61" s="74">
+        <v>0</v>
+      </c>
+      <c r="G61" s="74">
+        <v>0</v>
+      </c>
+      <c r="H61" s="74">
+        <v>0</v>
+      </c>
+      <c r="I61" s="74">
+        <v>0</v>
+      </c>
+      <c r="J61" s="74">
+        <v>0</v>
+      </c>
+      <c r="K61" s="74">
+        <v>0</v>
+      </c>
+      <c r="L61" s="74">
+        <v>0</v>
+      </c>
+      <c r="M61" s="74">
+        <v>0</v>
+      </c>
+      <c r="N61" s="74">
+        <v>0</v>
+      </c>
+      <c r="O61" s="74">
+        <v>0</v>
+      </c>
+      <c r="P61" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="39"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="74">
+        <v>0</v>
+      </c>
+      <c r="E62" s="74">
+        <v>0</v>
+      </c>
+      <c r="F62" s="74">
+        <v>0</v>
+      </c>
+      <c r="G62" s="74">
+        <v>0</v>
+      </c>
+      <c r="H62" s="74">
+        <v>0</v>
+      </c>
+      <c r="I62" s="74">
+        <v>0</v>
+      </c>
+      <c r="J62" s="74">
+        <v>0</v>
+      </c>
+      <c r="K62" s="74">
+        <v>0</v>
+      </c>
+      <c r="L62" s="74">
+        <v>0</v>
+      </c>
+      <c r="M62" s="74">
+        <v>0</v>
+      </c>
+      <c r="N62" s="74">
+        <v>0</v>
+      </c>
+      <c r="O62" s="74">
+        <v>0</v>
+      </c>
+      <c r="P62" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A63" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63" s="39"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="74">
+        <v>0</v>
+      </c>
+      <c r="E63" s="74">
+        <v>0</v>
+      </c>
+      <c r="F63" s="74">
+        <v>0</v>
+      </c>
+      <c r="G63" s="74">
+        <v>0</v>
+      </c>
+      <c r="H63" s="74">
+        <v>0</v>
+      </c>
+      <c r="I63" s="74">
+        <v>0</v>
+      </c>
+      <c r="J63" s="74">
+        <v>0</v>
+      </c>
+      <c r="K63" s="74">
+        <v>0</v>
+      </c>
+      <c r="L63" s="74">
+        <v>0</v>
+      </c>
+      <c r="M63" s="74">
+        <v>0</v>
+      </c>
+      <c r="N63" s="74">
+        <v>0</v>
+      </c>
+      <c r="O63" s="74">
+        <v>0</v>
+      </c>
+      <c r="P63" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A64" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" s="39"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="74">
+        <v>0</v>
+      </c>
+      <c r="E64" s="74">
+        <v>0</v>
+      </c>
+      <c r="F64" s="74">
+        <v>0</v>
+      </c>
+      <c r="G64" s="74">
+        <v>0</v>
+      </c>
+      <c r="H64" s="74">
+        <v>0</v>
+      </c>
+      <c r="I64" s="74">
+        <v>0</v>
+      </c>
+      <c r="J64" s="74">
+        <v>0</v>
+      </c>
+      <c r="K64" s="74">
+        <v>0</v>
+      </c>
+      <c r="L64" s="74">
+        <v>0</v>
+      </c>
+      <c r="M64" s="74">
+        <v>0</v>
+      </c>
+      <c r="N64" s="74">
+        <v>0</v>
+      </c>
+      <c r="O64" s="74">
+        <v>0</v>
+      </c>
+      <c r="P64" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A65" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="39"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="74">
+        <v>0</v>
+      </c>
+      <c r="E65" s="74">
+        <v>0</v>
+      </c>
+      <c r="F65" s="74">
+        <v>0</v>
+      </c>
+      <c r="G65" s="74">
+        <v>0</v>
+      </c>
+      <c r="H65" s="74">
+        <v>0</v>
+      </c>
+      <c r="I65" s="74">
+        <v>0</v>
+      </c>
+      <c r="J65" s="74">
+        <v>0</v>
+      </c>
+      <c r="K65" s="74">
+        <v>0</v>
+      </c>
+      <c r="L65" s="74">
+        <v>0</v>
+      </c>
+      <c r="M65" s="74">
+        <v>0</v>
+      </c>
+      <c r="N65" s="74">
+        <v>0</v>
+      </c>
+      <c r="O65" s="74">
+        <v>0</v>
+      </c>
+      <c r="P65" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A66" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66" s="39"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="74">
+        <v>0</v>
+      </c>
+      <c r="E66" s="74">
+        <v>0</v>
+      </c>
+      <c r="F66" s="74">
+        <v>0</v>
+      </c>
+      <c r="G66" s="74">
+        <v>0</v>
+      </c>
+      <c r="H66" s="74">
+        <v>0</v>
+      </c>
+      <c r="I66" s="74">
+        <v>0</v>
+      </c>
+      <c r="J66" s="74">
+        <v>0</v>
+      </c>
+      <c r="K66" s="74">
+        <v>0</v>
+      </c>
+      <c r="L66" s="74">
+        <v>0</v>
+      </c>
+      <c r="M66" s="74">
+        <v>0</v>
+      </c>
+      <c r="N66" s="74">
+        <v>0</v>
+      </c>
+      <c r="O66" s="74">
+        <v>0</v>
+      </c>
+      <c r="P66" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A67" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" s="39"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="74">
+        <v>0</v>
+      </c>
+      <c r="E67" s="74">
+        <v>0</v>
+      </c>
+      <c r="F67" s="74">
+        <v>0</v>
+      </c>
+      <c r="G67" s="74">
+        <v>0</v>
+      </c>
+      <c r="H67" s="74">
+        <v>0</v>
+      </c>
+      <c r="I67" s="74">
+        <v>0</v>
+      </c>
+      <c r="J67" s="74">
+        <v>0</v>
+      </c>
+      <c r="K67" s="74">
+        <v>0</v>
+      </c>
+      <c r="L67" s="74">
+        <v>0</v>
+      </c>
+      <c r="M67" s="74">
+        <v>0</v>
+      </c>
+      <c r="N67" s="74">
+        <v>0</v>
+      </c>
+      <c r="O67" s="74">
+        <v>0</v>
+      </c>
+      <c r="P67" s="74">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B68" s="42"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="76">
+        <v>0</v>
+      </c>
+      <c r="E68" s="76">
+        <v>0</v>
+      </c>
+      <c r="F68" s="76">
+        <v>0</v>
+      </c>
+      <c r="G68" s="76">
+        <v>0</v>
+      </c>
+      <c r="H68" s="76">
+        <v>0</v>
+      </c>
+      <c r="I68" s="76">
+        <v>0</v>
+      </c>
+      <c r="J68" s="76">
+        <v>0</v>
+      </c>
+      <c r="K68" s="76">
+        <v>0</v>
+      </c>
+      <c r="L68" s="76">
+        <v>0</v>
+      </c>
+      <c r="M68" s="76">
+        <v>0</v>
+      </c>
+      <c r="N68" s="76">
+        <v>0</v>
+      </c>
+      <c r="O68" s="76">
+        <v>0</v>
+      </c>
+      <c r="P68" s="76">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="46"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="H71" s="46"/>
+      <c r="I71" s="46"/>
+      <c r="J71" s="46"/>
+      <c r="K71" s="17"/>
+    </row>
+    <row r="72" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="52"/>
+      <c r="C72" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="F72" s="53"/>
+      <c r="G72" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="H72" s="52"/>
+      <c r="I72" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J72" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K72" s="55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A73" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" s="63"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="20">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0.81140000000000001</v>
+      </c>
+      <c r="F73" s="53"/>
+      <c r="G73" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="H73" s="63"/>
+      <c r="I73" s="20"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="5"/>
+    </row>
+    <row r="74" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A74" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" s="63"/>
+      <c r="C74" s="53"/>
+      <c r="D74" s="20">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="E74" s="5">
+        <v>0.82369999999999999</v>
+      </c>
+      <c r="F74" s="53"/>
+      <c r="G74" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="N48" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="O48" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="P48" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q48" s="64"/>
-    </row>
-    <row r="49" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="42"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="77">
-        <v>0</v>
-      </c>
-      <c r="E49" s="77">
-        <v>0</v>
-      </c>
-      <c r="F49" s="77">
-        <v>0</v>
-      </c>
-      <c r="G49" s="77">
-        <v>0</v>
-      </c>
-      <c r="H49" s="77">
-        <v>0</v>
-      </c>
-      <c r="I49" s="77">
-        <v>0</v>
-      </c>
-      <c r="J49" s="77">
-        <v>0</v>
-      </c>
-      <c r="K49" s="77">
-        <v>0</v>
-      </c>
-      <c r="L49" s="77">
-        <v>0</v>
-      </c>
-      <c r="M49" s="77">
-        <v>0</v>
-      </c>
-      <c r="N49" s="77">
-        <v>0</v>
-      </c>
-      <c r="O49" s="77">
-        <v>0</v>
-      </c>
-      <c r="P49" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="42"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="77">
-        <v>0</v>
-      </c>
-      <c r="E50" s="77">
-        <v>0</v>
-      </c>
-      <c r="F50" s="77">
-        <v>0</v>
-      </c>
-      <c r="G50" s="77">
-        <v>0</v>
-      </c>
-      <c r="H50" s="77">
-        <v>0</v>
-      </c>
-      <c r="I50" s="77">
-        <v>0</v>
-      </c>
-      <c r="J50" s="77">
-        <v>0</v>
-      </c>
-      <c r="K50" s="77">
-        <v>0</v>
-      </c>
-      <c r="L50" s="77">
-        <v>0</v>
-      </c>
-      <c r="M50" s="77">
-        <v>0</v>
-      </c>
-      <c r="N50" s="77">
-        <v>0</v>
-      </c>
-      <c r="O50" s="77">
-        <v>0</v>
-      </c>
-      <c r="P50" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" s="42"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="77">
-        <v>0</v>
-      </c>
-      <c r="E51" s="77">
-        <v>0</v>
-      </c>
-      <c r="F51" s="77">
-        <v>0</v>
-      </c>
-      <c r="G51" s="77">
-        <v>0</v>
-      </c>
-      <c r="H51" s="77">
-        <v>0</v>
-      </c>
-      <c r="I51" s="77">
-        <v>0</v>
-      </c>
-      <c r="J51" s="77">
-        <v>0</v>
-      </c>
-      <c r="K51" s="77">
-        <v>0</v>
-      </c>
-      <c r="L51" s="77">
-        <v>0</v>
-      </c>
-      <c r="M51" s="77">
-        <v>0</v>
-      </c>
-      <c r="N51" s="77">
-        <v>0</v>
-      </c>
-      <c r="O51" s="77">
-        <v>0</v>
-      </c>
-      <c r="P51" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="42"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="77">
-        <v>0</v>
-      </c>
-      <c r="E52" s="77">
-        <v>0</v>
-      </c>
-      <c r="F52" s="77">
-        <v>0</v>
-      </c>
-      <c r="G52" s="77">
-        <v>0</v>
-      </c>
-      <c r="H52" s="77">
-        <v>0</v>
-      </c>
-      <c r="I52" s="77">
-        <v>0</v>
-      </c>
-      <c r="J52" s="77">
-        <v>0</v>
-      </c>
-      <c r="K52" s="77">
-        <v>0</v>
-      </c>
-      <c r="L52" s="77">
-        <v>0</v>
-      </c>
-      <c r="M52" s="77">
-        <v>0</v>
-      </c>
-      <c r="N52" s="77">
-        <v>0</v>
-      </c>
-      <c r="O52" s="77">
-        <v>0</v>
-      </c>
-      <c r="P52" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="77">
-        <v>0</v>
-      </c>
-      <c r="E53" s="77">
-        <v>0</v>
-      </c>
-      <c r="F53" s="77">
-        <v>0</v>
-      </c>
-      <c r="G53" s="77">
-        <v>0</v>
-      </c>
-      <c r="H53" s="77">
-        <v>0</v>
-      </c>
-      <c r="I53" s="77">
-        <v>0</v>
-      </c>
-      <c r="J53" s="77">
-        <v>0</v>
-      </c>
-      <c r="K53" s="77">
-        <v>0</v>
-      </c>
-      <c r="L53" s="77">
-        <v>0</v>
-      </c>
-      <c r="M53" s="77">
-        <v>0</v>
-      </c>
-      <c r="N53" s="77">
-        <v>0</v>
-      </c>
-      <c r="O53" s="77">
-        <v>0</v>
-      </c>
-      <c r="P53" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="B54" s="42"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="77">
-        <v>0</v>
-      </c>
-      <c r="E54" s="77">
-        <v>0</v>
-      </c>
-      <c r="F54" s="77">
-        <v>0</v>
-      </c>
-      <c r="G54" s="77">
-        <v>0</v>
-      </c>
-      <c r="H54" s="77">
-        <v>0</v>
-      </c>
-      <c r="I54" s="77">
-        <v>0</v>
-      </c>
-      <c r="J54" s="77">
-        <v>0</v>
-      </c>
-      <c r="K54" s="77">
-        <v>0</v>
-      </c>
-      <c r="L54" s="77">
-        <v>0</v>
-      </c>
-      <c r="M54" s="77">
-        <v>0</v>
-      </c>
-      <c r="N54" s="77">
-        <v>0</v>
-      </c>
-      <c r="O54" s="77">
-        <v>0</v>
-      </c>
-      <c r="P54" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A55" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="B55" s="42"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="77">
-        <v>0</v>
-      </c>
-      <c r="E55" s="77">
-        <v>0</v>
-      </c>
-      <c r="F55" s="77">
-        <v>0</v>
-      </c>
-      <c r="G55" s="77">
-        <v>0</v>
-      </c>
-      <c r="H55" s="77">
-        <v>0</v>
-      </c>
-      <c r="I55" s="77">
-        <v>0</v>
-      </c>
-      <c r="J55" s="77">
-        <v>0</v>
-      </c>
-      <c r="K55" s="77">
-        <v>0</v>
-      </c>
-      <c r="L55" s="77">
-        <v>0</v>
-      </c>
-      <c r="M55" s="77">
-        <v>0</v>
-      </c>
-      <c r="N55" s="77">
-        <v>0</v>
-      </c>
-      <c r="O55" s="77">
-        <v>0</v>
-      </c>
-      <c r="P55" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="B56" s="42"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="77">
-        <v>0</v>
-      </c>
-      <c r="E56" s="77">
-        <v>0</v>
-      </c>
-      <c r="F56" s="77">
-        <v>0</v>
-      </c>
-      <c r="G56" s="77">
-        <v>0</v>
-      </c>
-      <c r="H56" s="77">
-        <v>0</v>
-      </c>
-      <c r="I56" s="77">
-        <v>0</v>
-      </c>
-      <c r="J56" s="77">
-        <v>0</v>
-      </c>
-      <c r="K56" s="77">
-        <v>0</v>
-      </c>
-      <c r="L56" s="77">
-        <v>0</v>
-      </c>
-      <c r="M56" s="77">
-        <v>0</v>
-      </c>
-      <c r="N56" s="77">
-        <v>0</v>
-      </c>
-      <c r="O56" s="77">
-        <v>0</v>
-      </c>
-      <c r="P56" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="B57" s="42"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="77">
-        <v>0</v>
-      </c>
-      <c r="E57" s="77">
-        <v>0</v>
-      </c>
-      <c r="F57" s="77">
-        <v>0</v>
-      </c>
-      <c r="G57" s="77">
-        <v>0</v>
-      </c>
-      <c r="H57" s="77">
-        <v>0</v>
-      </c>
-      <c r="I57" s="77">
-        <v>0</v>
-      </c>
-      <c r="J57" s="77">
-        <v>0</v>
-      </c>
-      <c r="K57" s="77">
-        <v>0</v>
-      </c>
-      <c r="L57" s="77">
-        <v>0</v>
-      </c>
-      <c r="M57" s="77">
-        <v>0</v>
-      </c>
-      <c r="N57" s="77">
-        <v>0</v>
-      </c>
-      <c r="O57" s="77">
-        <v>0</v>
-      </c>
-      <c r="P57" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B58" s="42"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="77">
-        <v>0</v>
-      </c>
-      <c r="E58" s="77">
-        <v>0</v>
-      </c>
-      <c r="F58" s="77">
-        <v>0</v>
-      </c>
-      <c r="G58" s="77">
-        <v>0</v>
-      </c>
-      <c r="H58" s="77">
-        <v>0</v>
-      </c>
-      <c r="I58" s="77">
-        <v>0</v>
-      </c>
-      <c r="J58" s="77">
-        <v>0</v>
-      </c>
-      <c r="K58" s="77">
-        <v>0</v>
-      </c>
-      <c r="L58" s="77">
-        <v>0</v>
-      </c>
-      <c r="M58" s="77">
-        <v>0</v>
-      </c>
-      <c r="N58" s="77">
-        <v>0</v>
-      </c>
-      <c r="O58" s="77">
-        <v>0</v>
-      </c>
-      <c r="P58" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q58" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="B59" s="42"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="77">
-        <v>0</v>
-      </c>
-      <c r="E59" s="77">
-        <v>0</v>
-      </c>
-      <c r="F59" s="77">
-        <v>0</v>
-      </c>
-      <c r="G59" s="77">
-        <v>0</v>
-      </c>
-      <c r="H59" s="77">
-        <v>0</v>
-      </c>
-      <c r="I59" s="77">
-        <v>0</v>
-      </c>
-      <c r="J59" s="77">
-        <v>0</v>
-      </c>
-      <c r="K59" s="77">
-        <v>0</v>
-      </c>
-      <c r="L59" s="77">
-        <v>0</v>
-      </c>
-      <c r="M59" s="77">
-        <v>0</v>
-      </c>
-      <c r="N59" s="77">
-        <v>0</v>
-      </c>
-      <c r="O59" s="77">
-        <v>0</v>
-      </c>
-      <c r="P59" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q59" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="77">
-        <v>0</v>
-      </c>
-      <c r="E60" s="77">
-        <v>0</v>
-      </c>
-      <c r="F60" s="77">
-        <v>0</v>
-      </c>
-      <c r="G60" s="77">
-        <v>0</v>
-      </c>
-      <c r="H60" s="77">
-        <v>0</v>
-      </c>
-      <c r="I60" s="77">
-        <v>0</v>
-      </c>
-      <c r="J60" s="77">
-        <v>0</v>
-      </c>
-      <c r="K60" s="77">
-        <v>0</v>
-      </c>
-      <c r="L60" s="77">
-        <v>0</v>
-      </c>
-      <c r="M60" s="77">
-        <v>0</v>
-      </c>
-      <c r="N60" s="77">
-        <v>0</v>
-      </c>
-      <c r="O60" s="77">
-        <v>0</v>
-      </c>
-      <c r="P60" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="77">
-        <v>0</v>
-      </c>
-      <c r="E61" s="77">
-        <v>0</v>
-      </c>
-      <c r="F61" s="77">
-        <v>0</v>
-      </c>
-      <c r="G61" s="77">
-        <v>0</v>
-      </c>
-      <c r="H61" s="77">
-        <v>0</v>
-      </c>
-      <c r="I61" s="77">
-        <v>0</v>
-      </c>
-      <c r="J61" s="77">
-        <v>0</v>
-      </c>
-      <c r="K61" s="77">
-        <v>0</v>
-      </c>
-      <c r="L61" s="77">
-        <v>0</v>
-      </c>
-      <c r="M61" s="77">
-        <v>0</v>
-      </c>
-      <c r="N61" s="77">
-        <v>0</v>
-      </c>
-      <c r="O61" s="77">
-        <v>0</v>
-      </c>
-      <c r="P61" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A62" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B62" s="42"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="77">
-        <v>0</v>
-      </c>
-      <c r="E62" s="77">
-        <v>0</v>
-      </c>
-      <c r="F62" s="77">
-        <v>0</v>
-      </c>
-      <c r="G62" s="77">
-        <v>0</v>
-      </c>
-      <c r="H62" s="77">
-        <v>0</v>
-      </c>
-      <c r="I62" s="77">
-        <v>0</v>
-      </c>
-      <c r="J62" s="77">
-        <v>0</v>
-      </c>
-      <c r="K62" s="77">
-        <v>0</v>
-      </c>
-      <c r="L62" s="77">
-        <v>0</v>
-      </c>
-      <c r="M62" s="77">
-        <v>0</v>
-      </c>
-      <c r="N62" s="77">
-        <v>0</v>
-      </c>
-      <c r="O62" s="77">
-        <v>0</v>
-      </c>
-      <c r="P62" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q62" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B63" s="42"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="77">
-        <v>0</v>
-      </c>
-      <c r="E63" s="77">
-        <v>0</v>
-      </c>
-      <c r="F63" s="77">
-        <v>0</v>
-      </c>
-      <c r="G63" s="77">
-        <v>0</v>
-      </c>
-      <c r="H63" s="77">
-        <v>0</v>
-      </c>
-      <c r="I63" s="77">
-        <v>0</v>
-      </c>
-      <c r="J63" s="77">
-        <v>0</v>
-      </c>
-      <c r="K63" s="77">
-        <v>0</v>
-      </c>
-      <c r="L63" s="77">
-        <v>0</v>
-      </c>
-      <c r="M63" s="77">
-        <v>0</v>
-      </c>
-      <c r="N63" s="77">
-        <v>0</v>
-      </c>
-      <c r="O63" s="77">
-        <v>0</v>
-      </c>
-      <c r="P63" s="77">
-        <v>0</v>
-      </c>
-      <c r="Q63" s="78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="B64" s="45"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="79">
-        <v>0</v>
-      </c>
-      <c r="E64" s="79">
-        <v>0</v>
-      </c>
-      <c r="F64" s="79">
-        <v>0</v>
-      </c>
-      <c r="G64" s="79">
-        <v>0</v>
-      </c>
-      <c r="H64" s="79">
-        <v>0</v>
-      </c>
-      <c r="I64" s="79">
-        <v>0</v>
-      </c>
-      <c r="J64" s="79">
-        <v>0</v>
-      </c>
-      <c r="K64" s="79">
-        <v>0</v>
-      </c>
-      <c r="L64" s="79">
-        <v>0</v>
-      </c>
-      <c r="M64" s="79">
-        <v>0</v>
-      </c>
-      <c r="N64" s="79">
-        <v>0</v>
-      </c>
-      <c r="O64" s="79">
-        <v>0</v>
-      </c>
-      <c r="P64" s="79">
-        <v>0</v>
-      </c>
-      <c r="Q64" s="80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="18" t="s">
+      <c r="H74" s="63"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="20"/>
+      <c r="K74" s="5"/>
+    </row>
+    <row r="75" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A75" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75" s="63"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="20">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="E75" s="5">
+        <v>0.80310000000000004</v>
+      </c>
+      <c r="F75" s="53"/>
+      <c r="G75" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="H75" s="63"/>
+      <c r="I75" s="20"/>
+      <c r="J75" s="20"/>
+      <c r="K75" s="5"/>
+    </row>
+    <row r="76" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B76" s="65"/>
+      <c r="C76" s="54"/>
+      <c r="D76" s="7">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="E76" s="8">
+        <v>0.82189999999999996</v>
+      </c>
+      <c r="F76" s="53"/>
+      <c r="G76" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="H76" s="65"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="8"/>
+    </row>
+    <row r="77" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A77" s="81"/>
+      <c r="B77" s="78"/>
+      <c r="C77" s="53"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="53"/>
+      <c r="G77" s="20"/>
+      <c r="H77" s="20"/>
+    </row>
+    <row r="78" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F78" s="53"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
+    </row>
+    <row r="79" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F79" s="53"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="20"/>
+    </row>
+    <row r="80" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A80" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="38"/>
-      <c r="G67" s="38"/>
-      <c r="H67" s="38"/>
-    </row>
-    <row r="68" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="53" t="s">
+      <c r="B80" s="80"/>
+      <c r="C80" s="80"/>
+      <c r="D80" s="83"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+    </row>
+    <row r="81" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="62"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D81" s="84"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="20"/>
+    </row>
+    <row r="82" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="55"/>
-      <c r="C68" s="17" t="s">
+      <c r="B82" s="51"/>
+      <c r="C82" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D82" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+    </row>
+    <row r="83" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A83" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" s="63"/>
+      <c r="C83" s="20">
+        <f xml:space="preserve"> D73 - B73</f>
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="D83" s="5">
+        <f>D73 - E73</f>
+        <v>3.0000000000000027E-3</v>
+      </c>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+    </row>
+    <row r="84" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A84" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B84" s="63"/>
+      <c r="C84" s="20">
+        <f>B74 - D74</f>
+        <v>-0.81440000000000001</v>
+      </c>
+      <c r="D84" s="5">
+        <f>E74 - D74</f>
+        <v>9.299999999999975E-3</v>
+      </c>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+    </row>
+    <row r="85" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A85" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="B85" s="63"/>
+      <c r="C85" s="20">
+        <f>D75 - B75</f>
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="D85" s="5">
+        <f xml:space="preserve"> D75 - E75</f>
+        <v>1.1299999999999977E-2</v>
+      </c>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="20"/>
+    </row>
+    <row r="86" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B86" s="65"/>
+      <c r="C86" s="7">
+        <f xml:space="preserve"> B76 - D76</f>
+        <v>-0.81440000000000001</v>
+      </c>
+      <c r="D86" s="8">
+        <f xml:space="preserve"> E76 - D76</f>
+        <v>7.4999999999999512E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E87" s="82"/>
+      <c r="F87" s="36"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="36"/>
+    </row>
+    <row r="88" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="37"/>
+    </row>
+    <row r="89" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A89" s="79" t="s">
+        <v>29</v>
+      </c>
+      <c r="B89" s="80"/>
+      <c r="C89" s="80"/>
+      <c r="D89" s="83"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="37"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="19"/>
+    </row>
+    <row r="90" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="62"/>
+      <c r="B90" s="63"/>
+      <c r="C90" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D68" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E68" s="58" t="s">
+      <c r="D90" s="84"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="53"/>
+      <c r="G90" s="20"/>
+      <c r="H90" s="20"/>
+    </row>
+    <row r="91" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="51"/>
+      <c r="C91" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F68" s="56"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
-    </row>
-    <row r="69" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B69" s="66"/>
-      <c r="C69" s="56"/>
-      <c r="D69" s="23">
-        <v>0.81440000000000001</v>
-      </c>
-      <c r="E69" s="5">
-        <v>0.81140000000000001</v>
-      </c>
-      <c r="F69" s="56"/>
-      <c r="G69" s="23"/>
-      <c r="H69" s="23"/>
-    </row>
-    <row r="70" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B70" s="66"/>
-      <c r="C70" s="56"/>
-      <c r="D70" s="23">
-        <v>0.81440000000000001</v>
-      </c>
-      <c r="E70" s="5">
-        <v>0.82369999999999999</v>
-      </c>
-      <c r="F70" s="56"/>
-      <c r="G70" s="23"/>
-      <c r="H70" s="23"/>
-    </row>
-    <row r="71" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A71" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="B71" s="66"/>
-      <c r="C71" s="56"/>
-      <c r="D71" s="23">
-        <v>0.81440000000000001</v>
-      </c>
-      <c r="E71" s="5">
-        <v>0.80310000000000004</v>
-      </c>
-      <c r="F71" s="56"/>
-      <c r="G71" s="23"/>
-      <c r="H71" s="23"/>
-    </row>
-    <row r="72" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B72" s="66"/>
-      <c r="C72" s="56"/>
-      <c r="D72" s="23">
-        <v>0.81440000000000001</v>
-      </c>
-      <c r="E72" s="5">
-        <v>0.82189999999999996</v>
-      </c>
-      <c r="F72" s="56"/>
-      <c r="G72" s="23"/>
-      <c r="H72" s="23"/>
-    </row>
-    <row r="73" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A73" s="65" t="s">
+      <c r="D91" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="E91" s="20"/>
+      <c r="F91" s="53"/>
+      <c r="G91" s="20"/>
+      <c r="H91" s="20"/>
+    </row>
+    <row r="92" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A92" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="66"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-      <c r="H73" s="23"/>
-    </row>
-    <row r="74" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="B74" s="66"/>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="23"/>
-      <c r="H74" s="23"/>
-    </row>
-    <row r="75" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B75" s="66"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="23"/>
-      <c r="G75" s="23"/>
-      <c r="H75" s="23"/>
-    </row>
-    <row r="76" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="B76" s="68"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="8"/>
-      <c r="F76" s="23"/>
-      <c r="G76" s="23"/>
-      <c r="H76" s="23"/>
-    </row>
-    <row r="77" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A77" s="81"/>
-      <c r="B77" s="81"/>
-      <c r="C77" s="23"/>
-      <c r="D77" s="23"/>
-      <c r="E77" s="23"/>
-      <c r="F77" s="23"/>
-      <c r="G77" s="23"/>
-      <c r="H77" s="23"/>
-    </row>
-    <row r="78" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A78" s="81"/>
-      <c r="B78" s="81"/>
-      <c r="C78" s="23"/>
-      <c r="D78" s="23"/>
-      <c r="E78" s="23"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="23"/>
-      <c r="H78" s="23"/>
-    </row>
-    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B80" s="84"/>
-      <c r="C80" s="84"/>
-      <c r="D80" s="85"/>
-      <c r="E80" s="82"/>
-      <c r="F80" s="39"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="39"/>
-    </row>
-    <row r="81" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="86"/>
-      <c r="B81" s="87"/>
-      <c r="C81" s="88" t="s">
-        <v>33</v>
-      </c>
-      <c r="D81" s="89"/>
-      <c r="E81" s="40"/>
-      <c r="F81" s="40"/>
-      <c r="G81" s="40"/>
-      <c r="H81" s="40"/>
-    </row>
-    <row r="82" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="86" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" s="87"/>
-      <c r="C82" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D82" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="E82" s="40"/>
-      <c r="F82" s="40"/>
-      <c r="G82" s="22"/>
-      <c r="H82" s="22"/>
-    </row>
-    <row r="83" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A83" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B83" s="66"/>
-      <c r="C83" s="23">
-        <f xml:space="preserve"> D69 - B69</f>
-        <v>0.81440000000000001</v>
-      </c>
-      <c r="D83" s="5">
-        <f>D69 - E69</f>
-        <v>3.0000000000000027E-3</v>
-      </c>
-      <c r="E83" s="23"/>
-      <c r="F83" s="56"/>
-      <c r="G83" s="23"/>
-      <c r="H83" s="23"/>
-    </row>
-    <row r="84" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A84" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="B84" s="66"/>
-      <c r="C84" s="23">
-        <f>B70 - D70</f>
-        <v>-0.81440000000000001</v>
-      </c>
-      <c r="D84" s="5">
-        <f>E70 - D70</f>
-        <v>9.299999999999975E-3</v>
-      </c>
-      <c r="E84" s="23"/>
-      <c r="F84" s="56"/>
-      <c r="G84" s="23"/>
-      <c r="H84" s="23"/>
-    </row>
-    <row r="85" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A85" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="B85" s="66"/>
-      <c r="C85" s="23">
-        <f>D71 - B71</f>
-        <v>0.81440000000000001</v>
-      </c>
-      <c r="D85" s="5">
-        <f xml:space="preserve"> D71 - E71</f>
-        <v>1.1299999999999977E-2</v>
-      </c>
-      <c r="E85" s="23"/>
-      <c r="F85" s="56"/>
-      <c r="G85" s="23"/>
-      <c r="H85" s="23"/>
-    </row>
-    <row r="86" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B86" s="66"/>
-      <c r="C86" s="23">
-        <f xml:space="preserve"> B72 - D72</f>
-        <v>-0.81440000000000001</v>
-      </c>
-      <c r="D86" s="5">
-        <f xml:space="preserve"> E72 - D72</f>
-        <v>7.4999999999999512E-3</v>
-      </c>
-      <c r="E86" s="23"/>
-      <c r="F86" s="56"/>
-      <c r="G86" s="23"/>
-      <c r="H86" s="23"/>
-    </row>
-    <row r="87" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="B87" s="66"/>
-      <c r="C87" s="56"/>
-      <c r="D87" s="75"/>
-      <c r="E87" s="56"/>
-      <c r="F87" s="56"/>
-    </row>
-    <row r="88" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="B88" s="66"/>
-      <c r="C88" s="56"/>
-      <c r="D88" s="75"/>
-      <c r="E88" s="56"/>
-      <c r="F88" s="56"/>
-    </row>
-    <row r="89" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B89" s="66"/>
-      <c r="C89" s="56"/>
-      <c r="D89" s="75"/>
-      <c r="E89" s="56"/>
-      <c r="F89" s="56"/>
-    </row>
-    <row r="90" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="B90" s="68"/>
-      <c r="C90" s="57"/>
-      <c r="D90" s="76"/>
-      <c r="E90" s="56"/>
-      <c r="F90" s="56"/>
+      <c r="B92" s="63"/>
+      <c r="C92" s="53"/>
+      <c r="D92" s="72"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="53"/>
+      <c r="G92" s="20"/>
+      <c r="H92" s="20"/>
+    </row>
+    <row r="93" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="B93" s="63"/>
+      <c r="C93" s="53"/>
+      <c r="D93" s="72"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="53"/>
+      <c r="G93" s="20"/>
+      <c r="H93" s="20"/>
+    </row>
+    <row r="94" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="B94" s="63"/>
+      <c r="C94" s="53"/>
+      <c r="D94" s="72"/>
+      <c r="E94" s="53"/>
+      <c r="F94" s="53"/>
+    </row>
+    <row r="95" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="B95" s="65"/>
+      <c r="C95" s="54"/>
+      <c r="D95" s="73"/>
+      <c r="E95" s="53"/>
+      <c r="F95" s="53"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C96" s="53"/>
+      <c r="D96" s="53"/>
+      <c r="E96" s="53"/>
+      <c r="F96" s="53"/>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C97" s="53"/>
+      <c r="D97" s="53"/>
+      <c r="E97" s="53"/>
+      <c r="F97" s="53"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
+  <mergeCells count="96">
+    <mergeCell ref="M22:R41"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
     <mergeCell ref="A83:B83"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G71:J71"/>
+    <mergeCell ref="P60:Q60"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="A73:B73"/>
     <mergeCell ref="A74:B74"/>
     <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A64:B64"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A59:D59"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A51:B51"/>
@@ -6396,8 +6573,9 @@
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="J21:K21"/>
     <mergeCell ref="A48:B48"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="L19:P38"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -6415,10 +6593,10 @@
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
     <mergeCell ref="Q16:S16"/>
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="Q12:S12"/>

</xml_diff>